<commit_message>
Genaue Kostenrechnung, mehr Infos zu Sensoren
</commit_message>
<xml_diff>
--- a/Formales/Kostenübersicht.xlsx
+++ b/Formales/Kostenübersicht.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bandle/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[Projects]\TUMLegoSegway.git\Formales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20160" yWindow="0" windowWidth="13440" windowHeight="20900" tabRatio="500"/>
+    <workbookView xWindow="20160" yWindow="0" windowWidth="13440" windowHeight="20895" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Genaue Kostenrechnung" sheetId="2" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Einzelteilübersicht</t>
   </si>
@@ -72,16 +73,119 @@
   </si>
   <si>
     <t>Option 2</t>
+  </si>
+  <si>
+    <t>PiStorms</t>
+  </si>
+  <si>
+    <t>http://www.mindsensors.com/ev3-and-nxt/17-glidewheel-as-angle-sensor-for-nxt-or-ev3</t>
+  </si>
+  <si>
+    <t>https://shop.lego.com/de-DE/EV3-Gyrosensor-45505</t>
+  </si>
+  <si>
+    <t>http://www.mindsensors.com/ev3-and-nxt/15-gyro-multisensitivity-accelerometer-and-compass-for-nxt-or-ev3</t>
+  </si>
+  <si>
+    <t>Gyro Sensor (Lego)</t>
+  </si>
+  <si>
+    <t>Gyro++ Sensor (MindSensors)</t>
+  </si>
+  <si>
+    <t>Angle Sensor (MindSensors)</t>
+  </si>
+  <si>
+    <t>http://www.mindsensors.com/stem-with-robotics/13-pistorms-v2-base-kit-raspberry-pi-brain-for-lego-robot</t>
+  </si>
+  <si>
+    <t>Einzelteile</t>
+  </si>
+  <si>
+    <t>https://www.dexterindustries.com/shop/brickpi-advanced-for-raspberry-pi/</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>MicroSD-Karte</t>
+  </si>
+  <si>
+    <t>Included: battery holder, frame</t>
+  </si>
+  <si>
+    <t>NOT included: gyro/angle sensor</t>
+  </si>
+  <si>
+    <t>HDMI cable</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/dp/B00BMKLVJ6?creative=165953&amp;creativeASIN=B00BMKLVJ6&amp;&amp;smid=A3JWKAKR8XB7XF&amp;tag=geizhalspre03-21</t>
+  </si>
+  <si>
+    <t>MicroUSB Power Supply</t>
+  </si>
+  <si>
+    <t>Included: touchscreen, frame</t>
+  </si>
+  <si>
+    <t>Option 1: Board</t>
+  </si>
+  <si>
+    <t>Benötigte Hardware</t>
+  </si>
+  <si>
+    <t>Option 2: Sensoren</t>
+  </si>
+  <si>
+    <t>Kosten</t>
+  </si>
+  <si>
+    <t>Notizen</t>
+  </si>
+  <si>
+    <t>Gesamtpreis</t>
+  </si>
+  <si>
+    <t>Einzelpreis</t>
+  </si>
+  <si>
+    <t>Versand fällt bei PiStorms weg</t>
+  </si>
+  <si>
+    <t>BrickPi + Lego gyro</t>
+  </si>
+  <si>
+    <t>BrickPi + Gyro++</t>
+  </si>
+  <si>
+    <t>PiStorms + Lego gyro</t>
+  </si>
+  <si>
+    <t>PiStorms + Gyro++ - shipping</t>
+  </si>
+  <si>
+    <t>PiStorms + Angle - shipping</t>
+  </si>
+  <si>
+    <t>Versand</t>
+  </si>
+  <si>
+    <t>BrickPi + Angle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ _€"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,8 +223,16 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,8 +245,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -230,11 +366,135 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -255,15 +515,65 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -532,26 +842,543 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.75" customWidth="1"/>
+    <col min="3" max="3" width="11.25" customWidth="1"/>
+    <col min="4" max="4" width="9.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.375" customWidth="1"/>
+    <col min="6" max="6" width="25.625" customWidth="1"/>
+    <col min="8" max="8" width="9.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="37">
+        <f>SUM(C2:D2)</f>
+        <v>100.50999999999999</v>
+      </c>
+      <c r="C2" s="37">
+        <v>60.66</v>
+      </c>
+      <c r="D2" s="48">
+        <v>39.85</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="16">
+        <f>SUM(C3:D3)</f>
+        <v>4</v>
+      </c>
+      <c r="C3" s="16">
+        <v>3</v>
+      </c>
+      <c r="D3" s="16">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16">
+        <f>SUM(C4:D4)</f>
+        <v>127.82000000000001</v>
+      </c>
+      <c r="C4" s="16">
+        <v>85.9</v>
+      </c>
+      <c r="D4" s="16">
+        <v>41.92</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="16">
+        <f>SUM(C5:D5)</f>
+        <v>310.95</v>
+      </c>
+      <c r="C5" s="16">
+        <v>293.95</v>
+      </c>
+      <c r="D5" s="16">
+        <v>17</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="16">
+        <f>SUM(C6:D6)</f>
+        <v>38.49</v>
+      </c>
+      <c r="C6" s="16">
+        <v>34.99</v>
+      </c>
+      <c r="D6" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="16">
+        <f>SUM(C7:D7)</f>
+        <v>96.960000000000008</v>
+      </c>
+      <c r="C7" s="16">
+        <v>57.11</v>
+      </c>
+      <c r="D7" s="49">
+        <v>39.85</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="16">
+        <f>SUM(C8:D8)</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="16">
+        <v>3</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="16">
+        <f>SUM(C9:D9)</f>
+        <v>7</v>
+      </c>
+      <c r="C9" s="16">
+        <v>6</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="16">
+        <f>SUM(C10:D10)</f>
+        <v>135.03</v>
+      </c>
+      <c r="C10" s="16">
+        <v>95.18</v>
+      </c>
+      <c r="D10" s="49">
+        <v>39.85</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="16">
+        <f>SUM(C11:D11)</f>
+        <v>6</v>
+      </c>
+      <c r="C11" s="16">
+        <v>5</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="36">
+        <f>SUM(C12:D12)</f>
+        <v>38.5</v>
+      </c>
+      <c r="C12" s="36">
+        <v>37.5</v>
+      </c>
+      <c r="D12" s="36">
+        <v>1</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="27"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="str">
+        <f>A5</f>
+        <v>EV3 Base Set</v>
+      </c>
+      <c r="B15" s="37">
+        <f>VLOOKUP($A15,$A$2:$B$12,2)</f>
+        <v>310.95</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="E15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="10">
+        <f>C$19+B$21+C25</f>
+        <v>533.76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="str">
+        <f>A12</f>
+        <v>Raspberry Pi 3</v>
+      </c>
+      <c r="B16" s="16">
+        <f>VLOOKUP($A16,$A$2:$B$12,2)</f>
+        <v>38.5</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="E16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="5">
+        <f>C$19+B$21+C26</f>
+        <v>592.23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="str">
+        <f>A9</f>
+        <v>MicroSD-Karte</v>
+      </c>
+      <c r="B17" s="16">
+        <f>VLOOKUP($A17,$A$2:$B$12,2)</f>
+        <v>7</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="E17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="5">
+        <f>C$19+B$21+C27</f>
+        <v>595.78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="str">
+        <f>A8</f>
+        <v>HDMI cable</v>
+      </c>
+      <c r="B18" s="16">
+        <f>VLOOKUP($A18,$A$2:$B$12,2)</f>
+        <v>4</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="str">
+        <f>A11</f>
+        <v>MicroUSB Power Supply</v>
+      </c>
+      <c r="B19" s="36">
+        <f>VLOOKUP($A19,$A$2:$B$12,2)</f>
+        <v>7</v>
+      </c>
+      <c r="C19" s="7">
+        <f>SUM(B15:B19)</f>
+        <v>367.45</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="5">
+        <f>C$19+C$23+C25</f>
+        <v>544.97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="52"/>
+      <c r="E20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="5">
+        <f>C$19+C$23+C26-D$10</f>
+        <v>563.59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="str">
+        <f>A4</f>
+        <v>BrickPi BaseKit</v>
+      </c>
+      <c r="B21" s="39">
+        <f>VLOOKUP($A21,$A$2:$B$12,2)</f>
+        <v>127.82000000000001</v>
+      </c>
+      <c r="C21" s="44">
+        <f>B21</f>
+        <v>127.82000000000001</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="7">
+        <f>C$19+C$23+C27-D$10</f>
+        <v>567.14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="str">
+        <f>A10</f>
+        <v>PiStorms</v>
+      </c>
+      <c r="B22" s="40">
+        <f>VLOOKUP($A22,$A$2:$B$12,2)</f>
+        <v>135.03</v>
+      </c>
+      <c r="C22" s="45"/>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="53" t="str">
+        <f>A3</f>
+        <v>Battery Holder</v>
+      </c>
+      <c r="B23" s="54">
+        <f>VLOOKUP($A23,$A$2:$B$12,2)</f>
+        <v>4</v>
+      </c>
+      <c r="C23" s="55">
+        <f>SUM(B22:B23)</f>
+        <v>139.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="43"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="str">
+        <f>A6</f>
+        <v>Gyro Sensor (Lego)</v>
+      </c>
+      <c r="B25" s="39">
+        <f>VLOOKUP($A25,$A$2:$B$12,2)</f>
+        <v>38.49</v>
+      </c>
+      <c r="C25" s="44">
+        <f>B25</f>
+        <v>38.49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="str">
+        <f>A7</f>
+        <v>Gyro++ Sensor (MindSensors)</v>
+      </c>
+      <c r="B26" s="41">
+        <f>VLOOKUP($A26,$A$2:$B$12,2)</f>
+        <v>96.960000000000008</v>
+      </c>
+      <c r="C26" s="46">
+        <f>B26</f>
+        <v>96.960000000000008</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="35" t="str">
+        <f>A2</f>
+        <v>Angle Sensor (MindSensors)</v>
+      </c>
+      <c r="B27" s="42">
+        <f>VLOOKUP($A27,$A$2:$B$12,2)</f>
+        <v>100.50999999999999</v>
+      </c>
+      <c r="C27" s="47">
+        <f>B27</f>
+        <v>100.50999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:G12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E10" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:3" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
@@ -559,7 +1386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -567,7 +1394,7 @@
         <v>60.66</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
@@ -575,7 +1402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -583,7 +1410,7 @@
         <v>85.9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -591,7 +1418,7 @@
         <v>293.95</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -599,7 +1426,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
@@ -607,7 +1434,7 @@
         <v>5.81</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
@@ -615,7 +1442,7 @@
         <v>95.18</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
@@ -623,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>3</v>
       </c>
@@ -631,14 +1458,14 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:3" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="13"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="str">
         <f>$B4</f>
         <v>Angle Sensor</v>
@@ -648,7 +1475,7 @@
         <v>60.66</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="str">
         <f>$B5</f>
         <v>Battery Holder</v>
@@ -658,7 +1485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="str">
         <f>$B6</f>
         <v>BrickPi BaseKit</v>
@@ -668,7 +1495,7 @@
         <v>85.9</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="str">
         <f>$B7</f>
         <v>EV3 Base Set</v>
@@ -678,7 +1505,7 @@
         <v>293.95</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="str">
         <f>$B8</f>
         <v>Gyro Sensor</v>
@@ -688,7 +1515,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="str">
         <f>$B11</f>
         <v>Power Supply</v>
@@ -698,7 +1525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>13</v>
       </c>
@@ -707,14 +1534,14 @@
         <v>483.5</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:3" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:3" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="13"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="str">
         <f>B4</f>
         <v>Angle Sensor</v>
@@ -724,7 +1551,7 @@
         <v>60.66</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="str">
         <f>B5</f>
         <v>Battery Holder</v>
@@ -734,7 +1561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="str">
         <f>B6</f>
         <v>BrickPi BaseKit</v>
@@ -744,7 +1571,7 @@
         <v>85.9</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="str">
         <f>B7</f>
         <v>EV3 Base Set</v>
@@ -754,7 +1581,7 @@
         <v>293.95</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="str">
         <f>B8</f>
         <v>Gyro Sensor</v>
@@ -764,7 +1591,7 @@
         <v>34.99</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="str">
         <f>B12</f>
         <v>Raspberry Pi 3</v>
@@ -774,7 +1601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
         <v>13</v>
       </c>

</xml_diff>